<commit_message>
Lots of results uploaded
</commit_message>
<xml_diff>
--- a/Python Algorithms/Microscopy_Sized_Results/data8_1002-data8_1010_p=S2/GFB-Critical.xlsx
+++ b/Python Algorithms/Microscopy_Sized_Results/data8_1002-data8_1010_p=S2/GFB-Critical.xlsx
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,22 +420,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>613</v>
+        <v>606</v>
       </c>
       <c r="C2">
-        <v>0.03253351214437653</v>
+        <v>0.03254204303681323</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>0.9993774050842392</v>
+        <v>0.9999016790546436</v>
       </c>
       <c r="F2">
-        <v>0.5502431392669678</v>
+        <v>0.09977054595947266</v>
       </c>
       <c r="G2">
-        <v>0.7729659505698775</v>
+        <v>0.7742536362831121</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -443,22 +443,160 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5670</v>
+        <v>5673</v>
       </c>
       <c r="C3">
-        <v>0.01789859065757605</v>
+        <v>0.01789872786270224</v>
       </c>
       <c r="D3">
         <v>0.1</v>
       </c>
       <c r="E3">
-        <v>0.09997462262294006</v>
+        <v>0.09998305469224604</v>
       </c>
       <c r="F3">
-        <v>3.257569074630737</v>
+        <v>0.7767543792724609</v>
       </c>
       <c r="G3">
-        <v>0.4429827322467485</v>
+        <v>0.4428740998807554</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>13767</v>
+      </c>
+      <c r="C4">
+        <v>0.01643449281948481</v>
+      </c>
+      <c r="D4">
+        <v>0.01</v>
+      </c>
+      <c r="E4">
+        <v>0.009997121167773834</v>
+      </c>
+      <c r="F4">
+        <v>1.899664402008057</v>
+      </c>
+      <c r="G4">
+        <v>0.3368040026290677</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>20622</v>
+      </c>
+      <c r="C5">
+        <v>0.01628805934426549</v>
+      </c>
+      <c r="D5">
+        <v>0.001</v>
+      </c>
+      <c r="E5">
+        <v>0.0009979150444940192</v>
+      </c>
+      <c r="F5">
+        <v>2.787895202636719</v>
+      </c>
+      <c r="G5">
+        <v>0.3163171269278453</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>21451</v>
+      </c>
+      <c r="C6">
+        <v>0.01627343664101082</v>
+      </c>
+      <c r="D6">
+        <v>0.0001</v>
+      </c>
+      <c r="E6">
+        <v>9.926314491103337E-05</v>
+      </c>
+      <c r="F6">
+        <v>2.893169164657593</v>
+      </c>
+      <c r="G6">
+        <v>0.3147820630490531</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>21504</v>
+      </c>
+      <c r="C7">
+        <v>0.01627195917621057</v>
+      </c>
+      <c r="D7">
+        <v>1E-05</v>
+      </c>
+      <c r="E7">
+        <v>8.464164299558957E-06</v>
+      </c>
+      <c r="F7">
+        <v>2.900102138519287</v>
+      </c>
+      <c r="G7">
+        <v>0.31469217492118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>22051</v>
+      </c>
+      <c r="C8">
+        <v>0.01627181648572707</v>
+      </c>
+      <c r="D8">
+        <v>1E-06</v>
+      </c>
+      <c r="E8">
+        <v>3.050127683218948E-07</v>
+      </c>
+      <c r="F8">
+        <v>2.969652414321899</v>
+      </c>
+      <c r="G8">
+        <v>0.3143282789609663</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>24802</v>
+      </c>
+      <c r="C9">
+        <v>0.01627182112465549</v>
+      </c>
+      <c r="D9">
+        <v>1E-07</v>
+      </c>
+      <c r="E9">
+        <v>1.992308490776627E-08</v>
+      </c>
+      <c r="F9">
+        <v>3.332269430160522</v>
+      </c>
+      <c r="G9">
+        <v>0.3143209987791079</v>
       </c>
     </row>
   </sheetData>

</xml_diff>